<commit_message>
upload mouse fasta files
</commit_message>
<xml_diff>
--- a/TableOfContents.xlsx
+++ b/TableOfContents.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xzhan50/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xzhan50/projects/shared_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFC5437-E8B9-D240-BD4A-FDC1295F6A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8C447A-290E-C044-92F7-906A126FA8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="6200" windowWidth="28040" windowHeight="17440" xr2:uid="{6411458D-589D-3B44-AD80-8E3620A75A15}"/>
+    <workbookView xWindow="10360" yWindow="3160" windowWidth="28040" windowHeight="17440" xr2:uid="{6411458D-589D-3B44-AD80-8E3620A75A15}"/>
   </bookViews>
   <sheets>
     <sheet name="content" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>paper link</t>
-  </si>
-  <si>
     <t>dash.csv</t>
   </si>
   <si>
@@ -66,6 +63,24 @@
   </si>
   <si>
     <t>read.csv("https://raw.githubusercontent.com/LarsenLab/shared_data/master/dash.csv", check.names = FALSE)</t>
+  </si>
+  <si>
+    <t>Db_P01899.fasta</t>
+  </si>
+  <si>
+    <t>Dd_P01900.fasta</t>
+  </si>
+  <si>
+    <t>Kb_P01901.fasta</t>
+  </si>
+  <si>
+    <t>Kd_P01902.fasta</t>
+  </si>
+  <si>
+    <t>web link</t>
+  </si>
+  <si>
+    <t>indirect predition, ms</t>
   </si>
 </sst>
 </file>
@@ -448,12 +463,12 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="23.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="28" style="1" customWidth="1"/>
     <col min="3" max="3" width="34.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="49" style="1" customWidth="1"/>
@@ -465,37 +480,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add dtables downloaded from www.proteinatlas.org
</commit_message>
<xml_diff>
--- a/TableOfContents.xlsx
+++ b/TableOfContents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xzhan50/projects/shared_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8C447A-290E-C044-92F7-906A126FA8F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB41D00-9169-C84B-9D0C-0CD7965980F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10360" yWindow="3160" windowWidth="28040" windowHeight="17440" xr2:uid="{6411458D-589D-3B44-AD80-8E3620A75A15}"/>
+    <workbookView xWindow="7480" yWindow="10260" windowWidth="28040" windowHeight="17440" xr2:uid="{6411458D-589D-3B44-AD80-8E3620A75A15}"/>
   </bookViews>
   <sheets>
     <sheet name="content" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -77,10 +77,19 @@
     <t>Kd_P01902.fasta</t>
   </si>
   <si>
-    <t>web link</t>
-  </si>
-  <si>
     <t>indirect predition, ms</t>
+  </si>
+  <si>
+    <t>https://www.proteinatlas.org/</t>
+  </si>
+  <si>
+    <t>web link/data source</t>
+  </si>
+  <si>
+    <t>HLA_aggregated.tsv</t>
+  </si>
+  <si>
+    <t>proteinatlas.tsv</t>
   </si>
 </sst>
 </file>
@@ -96,23 +105,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF222222"/>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,10 +151,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,7 +472,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D10" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -475,31 +484,31 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -508,7 +517,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -516,7 +525,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -524,7 +533,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -532,6 +541,22 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>